<commit_message>
query for item and embryo
</commit_message>
<xml_diff>
--- a/excel_templates/embryo_template.xlsx
+++ b/excel_templates/embryo_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ligangzhou/Money/rust/store-api/excel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FB8563-17C9-A04A-A94E-5D97F5D96AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5917F5-4F00-DF46-A835-1B91E4EFE02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="880" windowWidth="31540" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="产品列表" sheetId="1" r:id="rId1"/>
@@ -149,15 +149,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>444240</xdr:colOff>
+      <xdr:colOff>1192633</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>83622</xdr:rowOff>
+      <xdr:rowOff>94961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1097531</xdr:colOff>
+      <xdr:colOff>1845924</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1497315</xdr:rowOff>
+      <xdr:rowOff>1508654</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -186,7 +186,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="444240" y="271770"/>
+          <a:off x="1192633" y="287729"/>
           <a:ext cx="653291" cy="1413693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -199,22 +199,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>351518</xdr:colOff>
+      <xdr:colOff>1281339</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>249465</xdr:rowOff>
+      <xdr:rowOff>147411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1065893</xdr:colOff>
+      <xdr:colOff>2063750</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1795552</xdr:rowOff>
+      <xdr:rowOff>1840745</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA179895-60FD-DCA7-03A2-9A406B6A2149}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75561617-3599-8D56-D0D2-C6BB50C27BBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -236,8 +236,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="351518" y="2041072"/>
-          <a:ext cx="714375" cy="1546087"/>
+          <a:off x="1281339" y="1939018"/>
+          <a:ext cx="782411" cy="1693334"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -550,12 +550,12 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="46" customWidth="1"/>
     <col min="2" max="253" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>